<commit_message>
Update payment_terms_new from dashboard
</commit_message>
<xml_diff>
--- a/data/Long_Format_Payment_Terms.xlsx
+++ b/data/Long_Format_Payment_Terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\incaa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4549A2F1-1D3F-4863-9464-558973F0ABD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0868013A-A35E-AC4E-8C58-685DA91E43D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>KKA ARYA BAGIASTRA</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>PT Mipcon Konsultan Utama</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>PAGAR PANEL 310M (LAHAN BARU)</t>
+  </si>
+  <si>
+    <t>PAYMENT_DATE</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Koma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -726,25 +726,25 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="80.83203125" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -770,15 +770,15 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2" s="2">
         <v>45075</v>
@@ -802,12 +802,12 @@
         <v>45085</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="2">
         <v>45075</v>
@@ -831,12 +831,12 @@
         <v>45131</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>45075</v>
@@ -860,12 +860,12 @@
         <v>45149</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
       </c>
       <c r="C5" s="2">
         <v>45145</v>
@@ -889,12 +889,12 @@
         <v>45159</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
       <c r="C6" s="2">
         <v>45145</v>
@@ -918,9 +918,9 @@
         <v>45163</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -947,9 +947,9 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -976,9 +976,9 @@
         <v>45328</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1005,12 +1005,12 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2">
         <v>45145</v>
@@ -1034,12 +1034,12 @@
         <v>45124</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>45145</v>
@@ -1063,12 +1063,12 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2">
         <v>45145</v>
@@ -1092,12 +1092,12 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>45160</v>
@@ -1121,12 +1121,12 @@
         <v>45162</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <v>45160</v>
@@ -1150,12 +1150,12 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
         <v>45160</v>
@@ -1179,12 +1179,12 @@
         <v>45498</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <v>45160</v>
@@ -1208,12 +1208,12 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
       <c r="C17" s="2">
         <v>45200</v>
@@ -1237,12 +1237,12 @@
         <v>45253</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
         <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
       </c>
       <c r="C18" s="2">
         <v>45200</v>
@@ -1266,12 +1266,12 @@
         <v>45274</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
         <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
       </c>
       <c r="C19" s="2">
         <v>45200</v>
@@ -1295,12 +1295,12 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
       </c>
       <c r="C20" s="2">
         <v>45200</v>
@@ -1324,12 +1324,12 @@
         <v>45342</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
         <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
       </c>
       <c r="C21" s="2">
         <v>45200</v>
@@ -1353,12 +1353,12 @@
         <v>45384</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
       </c>
       <c r="C22" s="2">
         <v>45200</v>
@@ -1382,12 +1382,12 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
       </c>
       <c r="C23" s="2">
         <v>45200</v>
@@ -1411,12 +1411,12 @@
         <v>45420</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
         <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
       </c>
       <c r="C24" s="2">
         <v>45200</v>
@@ -1440,12 +1440,12 @@
         <v>45459</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
         <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
       </c>
       <c r="C25" s="2">
         <v>45200</v>
@@ -1469,12 +1469,12 @@
         <v>45465</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
       </c>
       <c r="C26" s="2">
         <v>45200</v>
@@ -1498,12 +1498,12 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
       </c>
       <c r="C27" s="2">
         <v>45200</v>
@@ -1527,12 +1527,12 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
         <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>33</v>
       </c>
       <c r="C28" s="2">
         <v>45200</v>
@@ -1556,12 +1556,12 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
         <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>33</v>
       </c>
       <c r="C29" s="2">
         <v>45200</v>
@@ -1585,12 +1585,12 @@
         <v>45602</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
         <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>33</v>
       </c>
       <c r="C30" s="2">
         <v>45200</v>
@@ -1614,12 +1614,12 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
         <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
       </c>
       <c r="C31" s="2">
         <v>45200</v>
@@ -1643,12 +1643,12 @@
         <v>45721</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
       </c>
       <c r="C32" s="2">
         <v>45200</v>
@@ -1672,12 +1672,12 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
       </c>
       <c r="C33" s="2">
         <v>45200</v>
@@ -1701,12 +1701,12 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
         <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
       </c>
       <c r="C34" s="2">
         <v>45200</v>
@@ -1730,12 +1730,12 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
         <v>32</v>
-      </c>
-      <c r="B35" t="s">
-        <v>33</v>
       </c>
       <c r="C35" s="2">
         <v>45200</v>
@@ -1759,12 +1759,12 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2">
         <v>45250</v>
@@ -1788,12 +1788,12 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="2">
         <v>45250</v>
@@ -1817,12 +1817,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2">
         <v>45250</v>
@@ -1846,12 +1846,12 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2">
         <v>45250</v>
@@ -1875,12 +1875,12 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="2">
         <v>45250</v>
@@ -1904,12 +1904,12 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2">
         <v>45250</v>
@@ -1933,12 +1933,12 @@
         <v>45582</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="2">
         <v>45250</v>
@@ -1962,12 +1962,12 @@
         <v>45618</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="2">
         <v>45250</v>
@@ -1991,12 +1991,12 @@
         <v>45649</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2">
         <v>45250</v>
@@ -2020,12 +2020,12 @@
         <v>45674</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="2">
         <v>45250</v>
@@ -2049,12 +2049,12 @@
         <v>45708</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="2">
         <v>45250</v>
@@ -2078,12 +2078,12 @@
         <v>45735</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2">
         <v>45250</v>
@@ -2107,12 +2107,12 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="2">
         <v>45250</v>
@@ -2136,12 +2136,12 @@
         <v>45799</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C49" s="2">
         <v>45250</v>
@@ -2165,12 +2165,12 @@
         <v>45827</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="2">
         <v>45250</v>
@@ -2194,12 +2194,12 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" s="2">
         <v>45250</v>
@@ -2223,12 +2223,12 @@
         <v>45896</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="2">
         <v>45314</v>
@@ -2252,12 +2252,12 @@
         <v>45316</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C53" s="2">
         <v>45314</v>
@@ -2281,12 +2281,12 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C54" s="2">
         <v>45314</v>
@@ -2310,12 +2310,12 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" s="2">
         <v>45314</v>
@@ -2339,12 +2339,12 @@
         <v>45695</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C56" s="2">
         <v>45455</v>
@@ -2368,12 +2368,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" s="2">
         <v>45455</v>
@@ -2397,12 +2397,12 @@
         <v>45622</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C58" s="2">
         <v>45455</v>
@@ -2426,12 +2426,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C59" s="2">
         <v>45455</v>
@@ -2455,12 +2455,12 @@
         <v>45849</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C60" s="2">
         <v>45455</v>
@@ -2484,12 +2484,12 @@
         <v>45849</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C61" s="2">
         <v>45455</v>
@@ -2513,12 +2513,12 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" t="s">
         <v>40</v>
-      </c>
-      <c r="B62" t="s">
-        <v>41</v>
       </c>
       <c r="C62" s="2">
         <v>45826</v>
@@ -2542,12 +2542,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
         <v>40</v>
-      </c>
-      <c r="B63" t="s">
-        <v>41</v>
       </c>
       <c r="C63" s="2">
         <v>45826</v>
@@ -2571,12 +2571,12 @@
         <v>45706</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C64" s="2">
         <v>45826</v>
@@ -2600,12 +2600,12 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C65" s="2">
         <v>45826</v>
@@ -2629,12 +2629,12 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C66" s="2">
         <v>45826</v>
@@ -2658,12 +2658,12 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C67" s="2">
         <v>45826</v>
@@ -2687,12 +2687,12 @@
         <v>45834</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C68" s="2">
         <v>45826</v>
@@ -2716,12 +2716,12 @@
         <v>45846</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C69" s="2">
         <v>45826</v>
@@ -2745,12 +2745,12 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" s="2">
         <v>45826</v>
@@ -2774,12 +2774,12 @@
         <v>45875</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C71" s="2">
         <v>45826</v>
@@ -2803,12 +2803,12 @@
         <v>45884</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C72" s="2">
         <v>45826</v>
@@ -2832,12 +2832,12 @@
         <v>45902</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C73" s="2">
         <v>45826</v>
@@ -2861,12 +2861,12 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C74" s="2">
         <v>45826</v>
@@ -2890,12 +2890,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C75" s="2">
         <v>45826</v>
@@ -2919,12 +2919,12 @@
         <v>45706</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C76" s="2">
         <v>45478</v>
@@ -2948,12 +2948,12 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C77" s="2">
         <v>45478</v>
@@ -2977,12 +2977,12 @@
         <v>45579</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C78" s="2">
         <v>45478</v>
@@ -3006,12 +3006,12 @@
         <v>45702</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C79" s="2">
         <v>45478</v>
@@ -3035,12 +3035,12 @@
         <v>45819</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C80" s="2">
         <v>45478</v>
@@ -3064,12 +3064,12 @@
         <v>45854</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C81" s="2">
         <v>45516</v>
@@ -3093,12 +3093,12 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C82" s="2">
         <v>45516</v>
@@ -3122,12 +3122,12 @@
         <v>45664</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C83" s="2">
         <v>45516</v>
@@ -3151,12 +3151,12 @@
         <v>45784</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C84" s="2">
         <v>45545</v>
@@ -3180,12 +3180,12 @@
         <v>45552</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C85" s="2">
         <v>45545</v>
@@ -3209,12 +3209,12 @@
         <v>45630</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C86" s="2">
         <v>45545</v>
@@ -3238,12 +3238,12 @@
         <v>45671</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C87" s="2">
         <v>45545</v>
@@ -3267,12 +3267,12 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C88" s="2">
         <v>45545</v>
@@ -3298,12 +3298,12 @@
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C89" s="2">
         <v>45545</v>
@@ -3329,12 +3329,12 @@
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" t="s">
         <v>47</v>
-      </c>
-      <c r="B90" t="s">
-        <v>48</v>
       </c>
       <c r="C90" s="2">
         <v>45474</v>
@@ -3360,12 +3360,12 @@
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" t="s">
         <v>47</v>
-      </c>
-      <c r="B91" t="s">
-        <v>48</v>
       </c>
       <c r="C91" s="2">
         <v>45474</v>
@@ -3391,12 +3391,12 @@
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>46</v>
+      </c>
+      <c r="B92" t="s">
         <v>47</v>
-      </c>
-      <c r="B92" t="s">
-        <v>48</v>
       </c>
       <c r="C92" s="2">
         <v>45474</v>
@@ -3422,12 +3422,12 @@
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="s">
         <v>47</v>
-      </c>
-      <c r="B93" t="s">
-        <v>48</v>
       </c>
       <c r="C93" s="2">
         <v>45474</v>
@@ -3453,12 +3453,12 @@
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>46</v>
+      </c>
+      <c r="B94" t="s">
         <v>47</v>
-      </c>
-      <c r="B94" t="s">
-        <v>48</v>
       </c>
       <c r="C94" s="2">
         <v>45474</v>
@@ -3484,12 +3484,12 @@
       <c r="N94" s="5"/>
       <c r="O94" s="5"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95" t="s">
         <v>47</v>
-      </c>
-      <c r="B95" t="s">
-        <v>48</v>
       </c>
       <c r="C95" s="2">
         <v>45474</v>
@@ -3515,12 +3515,12 @@
       <c r="N95" s="5"/>
       <c r="O95" s="5"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" t="s">
         <v>47</v>
-      </c>
-      <c r="B96" t="s">
-        <v>48</v>
       </c>
       <c r="C96" s="2">
         <v>45474</v>
@@ -3546,12 +3546,12 @@
       <c r="N96" s="5"/>
       <c r="O96" s="5"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>46</v>
+      </c>
+      <c r="B97" t="s">
         <v>47</v>
-      </c>
-      <c r="B97" t="s">
-        <v>48</v>
       </c>
       <c r="C97" s="2">
         <v>45474</v>
@@ -3577,12 +3577,12 @@
       <c r="N97" s="5"/>
       <c r="O97" s="5"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>46</v>
+      </c>
+      <c r="B98" t="s">
         <v>47</v>
-      </c>
-      <c r="B98" t="s">
-        <v>48</v>
       </c>
       <c r="C98" s="2">
         <v>45474</v>
@@ -3608,12 +3608,12 @@
       <c r="N98" s="5"/>
       <c r="O98" s="5"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B99" t="s">
         <v>47</v>
-      </c>
-      <c r="B99" t="s">
-        <v>48</v>
       </c>
       <c r="C99" s="2">
         <v>45474</v>
@@ -3639,12 +3639,12 @@
       <c r="N99" s="5"/>
       <c r="O99" s="5"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>46</v>
+      </c>
+      <c r="B100" t="s">
         <v>47</v>
-      </c>
-      <c r="B100" t="s">
-        <v>48</v>
       </c>
       <c r="C100" s="2">
         <v>45474</v>
@@ -3670,12 +3670,12 @@
       <c r="N100" s="5"/>
       <c r="O100" s="5"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>46</v>
+      </c>
+      <c r="B101" t="s">
         <v>47</v>
-      </c>
-      <c r="B101" t="s">
-        <v>48</v>
       </c>
       <c r="C101" s="2">
         <v>45474</v>
@@ -3701,12 +3701,12 @@
       <c r="N101" s="5"/>
       <c r="O101" s="5"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" t="s">
         <v>47</v>
-      </c>
-      <c r="B102" t="s">
-        <v>48</v>
       </c>
       <c r="C102" s="2">
         <v>45474</v>
@@ -3732,12 +3732,12 @@
       <c r="N102" s="5"/>
       <c r="O102" s="5"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>46</v>
+      </c>
+      <c r="B103" t="s">
         <v>47</v>
-      </c>
-      <c r="B103" t="s">
-        <v>48</v>
       </c>
       <c r="C103" s="2">
         <v>45474</v>
@@ -3763,12 +3763,12 @@
       <c r="N103" s="5"/>
       <c r="O103" s="5"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>46</v>
+      </c>
+      <c r="B104" t="s">
         <v>47</v>
-      </c>
-      <c r="B104" t="s">
-        <v>48</v>
       </c>
       <c r="C104" s="2">
         <v>45474</v>
@@ -3794,12 +3794,12 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
     </row>
-    <row r="105" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B105" t="s">
         <v>49</v>
-      </c>
-      <c r="B105" t="s">
-        <v>50</v>
       </c>
       <c r="C105" s="2">
         <v>45502</v>
@@ -3825,12 +3825,12 @@
       <c r="N105" s="5"/>
       <c r="O105" s="5"/>
     </row>
-    <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B106" t="s">
         <v>51</v>
-      </c>
-      <c r="B106" t="s">
-        <v>52</v>
       </c>
       <c r="C106" s="2">
         <v>45170</v>
@@ -3856,12 +3856,12 @@
       <c r="N106" s="5"/>
       <c r="O106" s="5"/>
     </row>
-    <row r="107" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B107" t="s">
         <v>53</v>
-      </c>
-      <c r="B107" t="s">
-        <v>54</v>
       </c>
       <c r="C107" s="2">
         <v>45574</v>
@@ -3887,12 +3887,12 @@
       <c r="N107" s="5"/>
       <c r="O107" s="5"/>
     </row>
-    <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B108" t="s">
         <v>55</v>
-      </c>
-      <c r="B108" t="s">
-        <v>56</v>
       </c>
       <c r="C108" s="2">
         <v>45583</v>
@@ -3918,12 +3918,12 @@
       <c r="N108" s="5"/>
       <c r="O108" s="5"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>54</v>
+      </c>
+      <c r="B109" t="s">
         <v>55</v>
-      </c>
-      <c r="B109" t="s">
-        <v>56</v>
       </c>
       <c r="C109" s="2">
         <v>45583</v>
@@ -3949,12 +3949,12 @@
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B110" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C110" s="2">
         <v>45589</v>
@@ -3980,12 +3980,12 @@
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C111" s="2">
         <v>45589</v>
@@ -4011,12 +4011,12 @@
       <c r="N111" s="5"/>
       <c r="O111" s="5"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>12</v>
       </c>
       <c r="B112" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C112" s="2">
         <v>45589</v>
@@ -4042,12 +4042,12 @@
       <c r="N112" s="5"/>
       <c r="O112" s="5"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>12</v>
       </c>
       <c r="B113" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C113" s="2">
         <v>45589</v>
@@ -4073,12 +4073,12 @@
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>12</v>
       </c>
       <c r="B114" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C114" s="2">
         <v>45589</v>
@@ -4104,12 +4104,12 @@
       <c r="N114" s="5"/>
       <c r="O114" s="5"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>12</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C115" s="2">
         <v>45589</v>
@@ -4135,12 +4135,12 @@
       <c r="N115" s="5"/>
       <c r="O115" s="5"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C116" s="2">
         <v>45589</v>
@@ -4166,12 +4166,12 @@
       <c r="N116" s="5"/>
       <c r="O116" s="5"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C117" s="2">
         <v>45589</v>
@@ -4197,12 +4197,12 @@
       <c r="N117" s="5"/>
       <c r="O117" s="5"/>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C118" s="2">
         <v>45589</v>
@@ -4228,12 +4228,12 @@
       <c r="N118" s="5"/>
       <c r="O118" s="5"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C119" s="2">
         <v>45666</v>
@@ -4261,12 +4261,12 @@
       <c r="N119" s="5"/>
       <c r="O119" s="5"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>24</v>
       </c>
       <c r="B120" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C120" s="2">
         <v>45666</v>
@@ -4294,12 +4294,12 @@
       <c r="N120" s="5"/>
       <c r="O120" s="5"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C121" s="2">
         <v>45638</v>
@@ -4325,12 +4325,12 @@
       <c r="N121" s="5"/>
       <c r="O121" s="5"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C122" s="2">
         <v>45638</v>
@@ -4356,12 +4356,12 @@
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C123" s="2">
         <v>45638</v>
@@ -4387,12 +4387,12 @@
       <c r="N123" s="5"/>
       <c r="O123" s="5"/>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B124" t="s">
         <v>58</v>
-      </c>
-      <c r="B124" t="s">
-        <v>59</v>
       </c>
       <c r="C124" s="2">
         <v>45646</v>
@@ -4418,12 +4418,12 @@
       <c r="N124" s="5"/>
       <c r="O124" s="5"/>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>57</v>
+      </c>
+      <c r="B125" t="s">
         <v>58</v>
-      </c>
-      <c r="B125" t="s">
-        <v>59</v>
       </c>
       <c r="C125" s="2">
         <v>45646</v>
@@ -4449,12 +4449,12 @@
       <c r="N125" s="5"/>
       <c r="O125" s="5"/>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>57</v>
+      </c>
+      <c r="B126" t="s">
         <v>58</v>
-      </c>
-      <c r="B126" t="s">
-        <v>59</v>
       </c>
       <c r="C126" s="2">
         <v>45646</v>
@@ -4480,12 +4480,12 @@
       <c r="N126" s="5"/>
       <c r="O126" s="5"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C127" s="2">
         <v>45636</v>
@@ -4511,12 +4511,12 @@
       <c r="N127" s="5"/>
       <c r="O127" s="5"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C128" s="2">
         <v>45636</v>
@@ -4542,12 +4542,12 @@
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C129" s="2">
         <v>45636</v>
@@ -4573,12 +4573,12 @@
       <c r="N129" s="5"/>
       <c r="O129" s="5"/>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C130" s="2">
         <v>45636</v>
@@ -4604,12 +4604,12 @@
       <c r="N130" s="5"/>
       <c r="O130" s="5"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C131" s="2">
         <v>45636</v>
@@ -4635,12 +4635,12 @@
       <c r="N131" s="5"/>
       <c r="O131" s="5"/>
     </row>
-    <row r="132" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C132" s="7">
         <v>45636</v>
@@ -4666,12 +4666,12 @@
       <c r="N132" s="9"/>
       <c r="O132" s="9"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B133" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C133" s="2">
         <v>45663</v>
@@ -4697,12 +4697,12 @@
       <c r="N133" s="5"/>
       <c r="O133" s="5"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>12</v>
       </c>
       <c r="B134" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C134" s="2">
         <v>45663</v>
@@ -4728,12 +4728,12 @@
       <c r="N134" s="5"/>
       <c r="O134" s="5"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B135" t="s">
         <v>63</v>
-      </c>
-      <c r="B135" t="s">
-        <v>64</v>
       </c>
       <c r="C135" s="2">
         <v>45663</v>
@@ -4759,12 +4759,12 @@
       <c r="N135" s="5"/>
       <c r="O135" s="5"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>62</v>
+      </c>
+      <c r="B136" t="s">
         <v>63</v>
-      </c>
-      <c r="B136" t="s">
-        <v>64</v>
       </c>
       <c r="C136" s="2">
         <v>45663</v>
@@ -4790,12 +4790,12 @@
       <c r="N136" s="5"/>
       <c r="O136" s="5"/>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>62</v>
+      </c>
+      <c r="B137" t="s">
         <v>63</v>
-      </c>
-      <c r="B137" t="s">
-        <v>64</v>
       </c>
       <c r="C137" s="2">
         <v>45663</v>
@@ -4821,12 +4821,12 @@
       <c r="N137" s="5"/>
       <c r="O137" s="5"/>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>62</v>
+      </c>
+      <c r="B138" t="s">
         <v>63</v>
-      </c>
-      <c r="B138" t="s">
-        <v>64</v>
       </c>
       <c r="C138" s="2">
         <v>45663</v>
@@ -4852,12 +4852,12 @@
       <c r="N138" s="5"/>
       <c r="O138" s="5"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>62</v>
+      </c>
+      <c r="B139" t="s">
         <v>63</v>
-      </c>
-      <c r="B139" t="s">
-        <v>64</v>
       </c>
       <c r="C139" s="2">
         <v>45663</v>
@@ -4883,12 +4883,12 @@
       <c r="N139" s="5"/>
       <c r="O139" s="5"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>62</v>
+      </c>
+      <c r="B140" t="s">
         <v>63</v>
-      </c>
-      <c r="B140" t="s">
-        <v>64</v>
       </c>
       <c r="C140" s="2">
         <v>45663</v>
@@ -4914,12 +4914,12 @@
       <c r="N140" s="5"/>
       <c r="O140" s="5"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>62</v>
+      </c>
+      <c r="B141" t="s">
         <v>63</v>
-      </c>
-      <c r="B141" t="s">
-        <v>64</v>
       </c>
       <c r="C141" s="2">
         <v>45663</v>
@@ -4945,12 +4945,12 @@
       <c r="N141" s="5"/>
       <c r="O141" s="5"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>62</v>
+      </c>
+      <c r="B142" t="s">
         <v>63</v>
-      </c>
-      <c r="B142" t="s">
-        <v>64</v>
       </c>
       <c r="C142" s="2">
         <v>45663</v>
@@ -4976,12 +4976,12 @@
       <c r="N142" s="5"/>
       <c r="O142" s="5"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B143" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C143" s="2">
         <v>45719</v>
@@ -5007,12 +5007,12 @@
       <c r="N143" s="5"/>
       <c r="O143" s="5"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C144" s="2">
         <v>45805</v>
@@ -5038,12 +5038,12 @@
       <c r="N144" s="5"/>
       <c r="O144" s="5"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>10</v>
       </c>
       <c r="B145" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C145" s="2">
         <v>45805</v>
@@ -5069,12 +5069,12 @@
       <c r="N145" s="5"/>
       <c r="O145" s="5"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>12</v>
       </c>
       <c r="B146" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C146" s="2">
         <v>45694</v>
@@ -5100,12 +5100,12 @@
       <c r="N146" s="5"/>
       <c r="O146" s="5"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>12</v>
       </c>
       <c r="B147" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C147" s="2">
         <v>45694</v>
@@ -5131,12 +5131,12 @@
       <c r="N147" s="5"/>
       <c r="O147" s="5"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>12</v>
       </c>
       <c r="B148" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C148" s="2">
         <v>45694</v>
@@ -5162,12 +5162,12 @@
       <c r="N148" s="5"/>
       <c r="O148" s="5"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>12</v>
       </c>
       <c r="B149" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C149" s="2">
         <v>45694</v>
@@ -5193,12 +5193,12 @@
       <c r="N149" s="5"/>
       <c r="O149" s="5"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>12</v>
       </c>
       <c r="B150" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C150" s="2">
         <v>45694</v>
@@ -5224,12 +5224,12 @@
       <c r="N150" s="5"/>
       <c r="O150" s="5"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C151" s="2">
         <v>45694</v>
@@ -5255,12 +5255,12 @@
       <c r="N151" s="5"/>
       <c r="O151" s="5"/>
     </row>
-    <row r="152" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B152" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C152" s="2">
         <v>45818</v>
@@ -5286,12 +5286,12 @@
       <c r="N152" s="5"/>
       <c r="O152" s="5"/>
     </row>
-    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B153" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C153" s="2">
         <v>45818</v>
@@ -5317,12 +5317,12 @@
       <c r="N153" s="5"/>
       <c r="O153" s="5"/>
     </row>
-    <row r="154" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B154" t="s">
         <v>69</v>
-      </c>
-      <c r="B154" t="s">
-        <v>70</v>
       </c>
       <c r="C154" s="2">
         <v>45778</v>
@@ -5348,12 +5348,12 @@
       <c r="N154" s="5"/>
       <c r="O154" s="5"/>
     </row>
-    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>68</v>
+      </c>
+      <c r="B155" t="s">
         <v>69</v>
-      </c>
-      <c r="B155" t="s">
-        <v>70</v>
       </c>
       <c r="C155" s="2">
         <v>45778</v>
@@ -5379,12 +5379,12 @@
       <c r="N155" s="5"/>
       <c r="O155" s="5"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>68</v>
+      </c>
+      <c r="B156" t="s">
         <v>69</v>
-      </c>
-      <c r="B156" t="s">
-        <v>70</v>
       </c>
       <c r="C156" s="2">
         <v>45778</v>
@@ -5410,12 +5410,12 @@
       <c r="N156" s="5"/>
       <c r="O156" s="5"/>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>68</v>
+      </c>
+      <c r="B157" t="s">
         <v>69</v>
-      </c>
-      <c r="B157" t="s">
-        <v>70</v>
       </c>
       <c r="C157" s="2">
         <v>45778</v>
@@ -5441,12 +5441,12 @@
       <c r="N157" s="5"/>
       <c r="O157" s="5"/>
     </row>
-    <row r="158" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B158" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C158" s="2">
         <v>45768</v>
@@ -5472,12 +5472,12 @@
       <c r="N158" s="5"/>
       <c r="O158" s="5"/>
     </row>
-    <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>14</v>
       </c>
       <c r="B159" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C159" s="2">
         <v>45768</v>
@@ -5503,12 +5503,12 @@
       <c r="N159" s="5"/>
       <c r="O159" s="5"/>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>14</v>
       </c>
       <c r="B160" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C160" s="2">
         <v>45768</v>
@@ -5534,12 +5534,12 @@
       <c r="N160" s="5"/>
       <c r="O160" s="5"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B161" t="s">
         <v>72</v>
-      </c>
-      <c r="B161" t="s">
-        <v>73</v>
       </c>
       <c r="C161" s="2">
         <v>45778</v>
@@ -5565,12 +5565,12 @@
       <c r="N161" s="5"/>
       <c r="O161" s="5"/>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>71</v>
+      </c>
+      <c r="B162" t="s">
         <v>72</v>
-      </c>
-      <c r="B162" t="s">
-        <v>73</v>
       </c>
       <c r="C162" s="2">
         <v>45778</v>
@@ -5596,12 +5596,12 @@
       <c r="N162" s="5"/>
       <c r="O162" s="5"/>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>71</v>
+      </c>
+      <c r="B163" t="s">
         <v>72</v>
-      </c>
-      <c r="B163" t="s">
-        <v>73</v>
       </c>
       <c r="C163" s="2">
         <v>45778</v>
@@ -5627,12 +5627,12 @@
       <c r="N163" s="5"/>
       <c r="O163" s="5"/>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>71</v>
+      </c>
+      <c r="B164" t="s">
         <v>72</v>
-      </c>
-      <c r="B164" t="s">
-        <v>73</v>
       </c>
       <c r="C164" s="2">
         <v>45778</v>
@@ -5658,12 +5658,12 @@
       <c r="N164" s="5"/>
       <c r="O164" s="5"/>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>71</v>
+      </c>
+      <c r="B165" t="s">
         <v>72</v>
-      </c>
-      <c r="B165" t="s">
-        <v>73</v>
       </c>
       <c r="C165" s="2">
         <v>45778</v>
@@ -5689,12 +5689,12 @@
       <c r="N165" s="5"/>
       <c r="O165" s="5"/>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>71</v>
+      </c>
+      <c r="B166" t="s">
         <v>72</v>
-      </c>
-      <c r="B166" t="s">
-        <v>73</v>
       </c>
       <c r="C166" s="2">
         <v>45778</v>
@@ -5720,12 +5720,12 @@
       <c r="N166" s="5"/>
       <c r="O166" s="5"/>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>71</v>
+      </c>
+      <c r="B167" t="s">
         <v>72</v>
-      </c>
-      <c r="B167" t="s">
-        <v>73</v>
       </c>
       <c r="C167" s="2">
         <v>45778</v>
@@ -5751,12 +5751,12 @@
       <c r="N167" s="5"/>
       <c r="O167" s="5"/>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>71</v>
+      </c>
+      <c r="B168" t="s">
         <v>72</v>
-      </c>
-      <c r="B168" t="s">
-        <v>73</v>
       </c>
       <c r="C168" s="2">
         <v>45778</v>
@@ -5782,12 +5782,12 @@
       <c r="N168" s="5"/>
       <c r="O168" s="5"/>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>71</v>
+      </c>
+      <c r="B169" t="s">
         <v>72</v>
-      </c>
-      <c r="B169" t="s">
-        <v>73</v>
       </c>
       <c r="C169" s="2">
         <v>45778</v>
@@ -5813,12 +5813,12 @@
       <c r="N169" s="5"/>
       <c r="O169" s="5"/>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>71</v>
+      </c>
+      <c r="B170" t="s">
         <v>72</v>
-      </c>
-      <c r="B170" t="s">
-        <v>73</v>
       </c>
       <c r="C170" s="2">
         <v>45778</v>
@@ -5844,12 +5844,12 @@
       <c r="N170" s="5"/>
       <c r="O170" s="5"/>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>71</v>
+      </c>
+      <c r="B171" t="s">
         <v>72</v>
-      </c>
-      <c r="B171" t="s">
-        <v>73</v>
       </c>
       <c r="C171" s="2">
         <v>45778</v>
@@ -5875,12 +5875,12 @@
       <c r="N171" s="5"/>
       <c r="O171" s="5"/>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>71</v>
+      </c>
+      <c r="B172" t="s">
         <v>72</v>
-      </c>
-      <c r="B172" t="s">
-        <v>73</v>
       </c>
       <c r="C172" s="2">
         <v>45778</v>
@@ -5906,12 +5906,12 @@
       <c r="N172" s="5"/>
       <c r="O172" s="5"/>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>71</v>
+      </c>
+      <c r="B173" t="s">
         <v>72</v>
-      </c>
-      <c r="B173" t="s">
-        <v>73</v>
       </c>
       <c r="C173" s="2">
         <v>45778</v>
@@ -5937,12 +5937,12 @@
       <c r="N173" s="5"/>
       <c r="O173" s="5"/>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>71</v>
+      </c>
+      <c r="B174" t="s">
         <v>72</v>
-      </c>
-      <c r="B174" t="s">
-        <v>73</v>
       </c>
       <c r="C174" s="2">
         <v>45778</v>
@@ -5968,12 +5968,12 @@
       <c r="N174" s="5"/>
       <c r="O174" s="5"/>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B175" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C175" s="2">
         <v>45834</v>
@@ -5999,12 +5999,12 @@
       <c r="N175" s="5"/>
       <c r="O175" s="5"/>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>9</v>
       </c>
       <c r="B176" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C176" s="2">
         <v>45834</v>
@@ -6030,9 +6030,9 @@
       <c r="N176" s="5"/>
       <c r="O176" s="5"/>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B177" t="s">
         <v>19</v>
@@ -6061,9 +6061,9 @@
       <c r="N177" s="5"/>
       <c r="O177" s="5"/>
     </row>
-    <row r="178" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B178" t="s">
         <v>20</v>
@@ -6092,7 +6092,7 @@
       <c r="N178" s="5"/>
       <c r="O178" s="5"/>
     </row>
-    <row r="179" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>12</v>
       </c>
@@ -6123,12 +6123,12 @@
       <c r="N179" s="5"/>
       <c r="O179" s="5"/>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>10</v>
       </c>
       <c r="B180" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C180" s="2">
         <v>45852</v>
@@ -6155,12 +6155,12 @@
       <c r="N180" s="5"/>
       <c r="O180" s="5"/>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>10</v>
       </c>
       <c r="B181" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C181" s="2">
         <v>45852</v>
@@ -6187,12 +6187,12 @@
       <c r="N181" s="5"/>
       <c r="O181" s="5"/>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B182" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C182" s="2">
         <v>45845</v>
@@ -6218,12 +6218,12 @@
       <c r="N182" s="5"/>
       <c r="O182" s="5"/>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>22</v>
       </c>
       <c r="B183" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C183" s="2">
         <v>45845</v>
@@ -6249,12 +6249,12 @@
       <c r="N183" s="5"/>
       <c r="O183" s="5"/>
     </row>
-    <row r="184" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>22</v>
       </c>
       <c r="B184" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C184" s="2">
         <v>45901</v>
@@ -6280,12 +6280,12 @@
       <c r="N184" s="5"/>
       <c r="O184" s="5"/>
     </row>
-    <row r="185" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>22</v>
       </c>
       <c r="B185" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C185" s="2">
         <v>45901</v>
@@ -6312,12 +6312,12 @@
       <c r="N185" s="5"/>
       <c r="O185" s="5"/>
     </row>
-    <row r="186" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>22</v>
       </c>
       <c r="B186" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C186" s="2">
         <v>45888</v>
@@ -6330,18 +6330,18 @@
       </c>
       <c r="G186" s="3"/>
       <c r="H186" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I186" s="2"/>
       <c r="N186" s="5"/>
       <c r="O186" s="5"/>
     </row>
-    <row r="187" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>23</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C187" s="2">
         <v>45883</v>
@@ -6367,12 +6367,12 @@
       <c r="N187" s="5"/>
       <c r="O187" s="5"/>
     </row>
-    <row r="188" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>23</v>
       </c>
       <c r="B188" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C188" s="2">
         <v>45883</v>
@@ -6398,12 +6398,12 @@
       <c r="N188" s="5"/>
       <c r="O188" s="5"/>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>83</v>
+      </c>
+      <c r="B189" t="s">
         <v>84</v>
-      </c>
-      <c r="B189" t="s">
-        <v>85</v>
       </c>
       <c r="C189" s="2">
         <v>45867</v>
@@ -6427,12 +6427,12 @@
         <v>45862</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>22</v>
       </c>
       <c r="B190" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C190" s="2">
         <v>45888</v>
@@ -6456,12 +6456,12 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>9</v>
       </c>
       <c r="B191" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C191" s="2">
         <v>45905</v>
@@ -6485,12 +6485,12 @@
         <v>45904</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>9</v>
       </c>
       <c r="B192" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C192" s="2">
         <v>45905</v>
@@ -6514,12 +6514,12 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B193" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C193" s="2">
         <v>45895</v>
@@ -6544,12 +6544,12 @@
         <v>45924</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>9</v>
       </c>
       <c r="B194" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C194" s="2">
         <v>45923</v>
@@ -6573,12 +6573,12 @@
         <v>45925</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>9</v>
       </c>
       <c r="B195" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C195" s="2">
         <v>45905</v>
@@ -6593,15 +6593,15 @@
         <v>1</v>
       </c>
       <c r="H195" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>9</v>
       </c>
       <c r="B196" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C196" s="2">
         <v>45905</v>
@@ -6622,12 +6622,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>9</v>
       </c>
       <c r="B197" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C197" s="2">
         <v>45905</v>
@@ -6672,43 +6672,43 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>84904</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>51512</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>49667</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>SUM(A1:A3)</f>
         <v>186083</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>122202733732</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>126971710115</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <f>A7-A6</f>
         <v>4768976383</v>

</xml_diff>

<commit_message>
Update data/Long_Format_Payment_Terms.xlsx via dashboard
</commit_message>
<xml_diff>
--- a/data/Long_Format_Payment_Terms.xlsx
+++ b/data/Long_Format_Payment_Terms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data Kerja INA\2025\1. Monthly Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76333265-5343-429B-8B95-B8B2E8C6BF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE5B82C-FBF4-9E40-9437-5BE6AF479FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Koma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -738,28 +738,28 @@
   <dimension ref="A1:O239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C195" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G223" sqref="G223"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.109375" customWidth="1"/>
-    <col min="2" max="2" width="80.88671875" customWidth="1"/>
+    <col min="1" max="1" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="80.83203125" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
@@ -811,13 +811,13 @@
         <v>131619360</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2">
         <v>45085</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -846,7 +846,7 @@
         <v>45131</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -875,7 +875,7 @@
         <v>45149</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -904,7 +904,7 @@
         <v>45159</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -933,7 +933,7 @@
         <v>45163</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -962,7 +962,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -991,7 +991,7 @@
         <v>45328</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>45436</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>45124</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>45162</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>45498</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>45253</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>45274</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>45307</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>45342</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>45384</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>45420</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>45459</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>45465</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>45620</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>45602</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>45721</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>45864</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>8</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>8</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>8</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>45538</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>8</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>45582</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>8</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>45618</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>8</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>45649</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>45674</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>45708</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>8</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>45735</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>8</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>8</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>45799</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>8</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>45827</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>45896</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>8</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>45936</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>8</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>11</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>45316</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>45345</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>45558</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>45695</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>45964</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>15</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>45622</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>45849</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>45849</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>45897</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>40</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>45706</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>40</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>45810</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>45820</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>40</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>45834</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>40</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>45846</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>40</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>45863</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>45875</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>40</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>45884</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>40</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>45902</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>40</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>40</v>
       </c>
@@ -3195,7 +3195,7 @@
         <v>45938</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>40</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>45951</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>40</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>45972</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>40</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>40</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>40</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>45706</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>7</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>45478</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>45579</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>45702</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>45819</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>45989</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>13</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>45664</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>13</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>45784</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>9</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>45552</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -3630,7 +3630,7 @@
         <v>45630</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>45671</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -3719,7 +3719,7 @@
       <c r="N102" s="5"/>
       <c r="O102" s="5"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -3750,7 +3750,7 @@
       <c r="N103" s="5"/>
       <c r="O103" s="5"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -3781,7 +3781,7 @@
       <c r="N104" s="5"/>
       <c r="O104" s="5"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>47</v>
       </c>
@@ -3812,7 +3812,7 @@
       <c r="N105" s="5"/>
       <c r="O105" s="5"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>47</v>
       </c>
@@ -3843,7 +3843,7 @@
       <c r="N106" s="5"/>
       <c r="O106" s="5"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="N107" s="5"/>
       <c r="O107" s="5"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>47</v>
       </c>
@@ -3905,7 +3905,7 @@
       <c r="N108" s="5"/>
       <c r="O108" s="5"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>47</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="N109" s="5"/>
       <c r="O109" s="5"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>47</v>
       </c>
@@ -3967,7 +3967,7 @@
       <c r="N110" s="5"/>
       <c r="O110" s="5"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="N111" s="5"/>
       <c r="O111" s="5"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -4029,7 +4029,7 @@
       <c r="N112" s="5"/>
       <c r="O112" s="5"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>47</v>
       </c>
@@ -4060,7 +4060,7 @@
       <c r="N113" s="5"/>
       <c r="O113" s="5"/>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>47</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="N114" s="5"/>
       <c r="O114" s="5"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>47</v>
       </c>
@@ -4122,7 +4122,7 @@
       <c r="N115" s="5"/>
       <c r="O115" s="5"/>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>47</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="N116" s="5"/>
       <c r="O116" s="5"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>47</v>
       </c>
@@ -4184,7 +4184,7 @@
       <c r="N117" s="5"/>
       <c r="O117" s="5"/>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>47</v>
       </c>
@@ -4215,7 +4215,7 @@
       <c r="N118" s="5"/>
       <c r="O118" s="5"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>47</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="N119" s="5"/>
       <c r="O119" s="5"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>47</v>
       </c>
@@ -4277,7 +4277,7 @@
       <c r="N120" s="5"/>
       <c r="O120" s="5"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>47</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="N121" s="5"/>
       <c r="O121" s="5"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>47</v>
       </c>
@@ -4339,7 +4339,7 @@
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
     </row>
-    <row r="123" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>49</v>
       </c>
@@ -4370,7 +4370,7 @@
       <c r="N123" s="5"/>
       <c r="O123" s="5"/>
     </row>
-    <row r="124" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>51</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="N124" s="5"/>
       <c r="O124" s="5"/>
     </row>
-    <row r="125" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>53</v>
       </c>
@@ -4432,7 +4432,7 @@
       <c r="N125" s="5"/>
       <c r="O125" s="5"/>
     </row>
-    <row r="126" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>55</v>
       </c>
@@ -4463,7 +4463,7 @@
       <c r="N126" s="5"/>
       <c r="O126" s="5"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>55</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="N127" s="5"/>
       <c r="O127" s="5"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
         <v>12</v>
       </c>
@@ -4525,7 +4525,7 @@
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>12</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="N129" s="5"/>
       <c r="O129" s="5"/>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>12</v>
       </c>
@@ -4587,7 +4587,7 @@
       <c r="N130" s="5"/>
       <c r="O130" s="5"/>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>12</v>
       </c>
@@ -4618,7 +4618,7 @@
       <c r="N131" s="5"/>
       <c r="O131" s="5"/>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>12</v>
       </c>
@@ -4649,7 +4649,7 @@
       <c r="N132" s="5"/>
       <c r="O132" s="5"/>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>12</v>
       </c>
@@ -4680,7 +4680,7 @@
       <c r="N133" s="5"/>
       <c r="O133" s="5"/>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>12</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="N134" s="5"/>
       <c r="O134" s="5"/>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -4742,7 +4742,7 @@
       <c r="N135" s="5"/>
       <c r="O135" s="5"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>12</v>
       </c>
@@ -4773,7 +4773,7 @@
       <c r="N136" s="5"/>
       <c r="O136" s="5"/>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>12</v>
       </c>
@@ -4801,7 +4801,7 @@
       <c r="N137" s="5"/>
       <c r="O137" s="5"/>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>12</v>
       </c>
@@ -4829,7 +4829,7 @@
       <c r="N138" s="5"/>
       <c r="O138" s="5"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>24</v>
       </c>
@@ -4862,7 +4862,7 @@
       <c r="N139" s="5"/>
       <c r="O139" s="5"/>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -4895,7 +4895,7 @@
       <c r="N140" s="5"/>
       <c r="O140" s="5"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>10</v>
       </c>
@@ -4926,7 +4926,7 @@
       <c r="N141" s="5"/>
       <c r="O141" s="5"/>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -4957,7 +4957,7 @@
       <c r="N142" s="5"/>
       <c r="O142" s="5"/>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>10</v>
       </c>
@@ -4988,7 +4988,7 @@
       <c r="N143" s="5"/>
       <c r="O143" s="5"/>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>58</v>
       </c>
@@ -5019,7 +5019,7 @@
       <c r="N144" s="5"/>
       <c r="O144" s="5"/>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>58</v>
       </c>
@@ -5050,7 +5050,7 @@
       <c r="N145" s="5"/>
       <c r="O145" s="5"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>58</v>
       </c>
@@ -5081,7 +5081,7 @@
       <c r="N146" s="5"/>
       <c r="O146" s="5"/>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" s="7" t="s">
         <v>11</v>
       </c>
@@ -5112,7 +5112,7 @@
       <c r="N147" s="5"/>
       <c r="O147" s="5"/>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -5143,7 +5143,7 @@
       <c r="N148" s="5"/>
       <c r="O148" s="5"/>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -5174,7 +5174,7 @@
       <c r="N149" s="5"/>
       <c r="O149" s="5"/>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -5205,7 +5205,7 @@
       <c r="N150" s="5"/>
       <c r="O150" s="5"/>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -5236,7 +5236,7 @@
       <c r="N151" s="5"/>
       <c r="O151" s="5"/>
     </row>
-    <row r="152" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
         <v>11</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="N152" s="12"/>
       <c r="O152" s="12"/>
     </row>
-    <row r="153" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="9" t="s">
         <v>11</v>
       </c>
@@ -5298,7 +5298,7 @@
       <c r="N153" s="12"/>
       <c r="O153" s="12"/>
     </row>
-    <row r="154" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="9" t="s">
         <v>11</v>
       </c>
@@ -5329,7 +5329,7 @@
       <c r="N154" s="12"/>
       <c r="O154" s="12"/>
     </row>
-    <row r="155" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="9" t="s">
         <v>11</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="N155" s="12"/>
       <c r="O155" s="12"/>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" s="7" t="s">
         <v>12</v>
       </c>
@@ -5391,7 +5391,7 @@
       <c r="N156" s="5"/>
       <c r="O156" s="5"/>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>12</v>
       </c>
@@ -5422,7 +5422,7 @@
       <c r="N157" s="5"/>
       <c r="O157" s="5"/>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>12</v>
       </c>
@@ -5453,7 +5453,7 @@
       <c r="N158" s="5"/>
       <c r="O158" s="5"/>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" s="7" t="s">
         <v>63</v>
       </c>
@@ -5484,7 +5484,7 @@
       <c r="N159" s="5"/>
       <c r="O159" s="5"/>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>63</v>
       </c>
@@ -5515,7 +5515,7 @@
       <c r="N160" s="5"/>
       <c r="O160" s="5"/>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>63</v>
       </c>
@@ -5546,7 +5546,7 @@
       <c r="N161" s="5"/>
       <c r="O161" s="5"/>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>63</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="N162" s="5"/>
       <c r="O162" s="5"/>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>63</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="N163" s="5"/>
       <c r="O163" s="5"/>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>63</v>
       </c>
@@ -5639,7 +5639,7 @@
       <c r="N164" s="5"/>
       <c r="O164" s="5"/>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>63</v>
       </c>
@@ -5670,7 +5670,7 @@
       <c r="N165" s="5"/>
       <c r="O165" s="5"/>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>63</v>
       </c>
@@ -5701,7 +5701,7 @@
       <c r="N166" s="5"/>
       <c r="O166" s="5"/>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>63</v>
       </c>
@@ -5732,7 +5732,7 @@
       <c r="N167" s="5"/>
       <c r="O167" s="5"/>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>63</v>
       </c>
@@ -5763,7 +5763,7 @@
       <c r="N168" s="5"/>
       <c r="O168" s="5"/>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>49</v>
       </c>
@@ -5794,7 +5794,7 @@
       <c r="N169" s="5"/>
       <c r="O169" s="5"/>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -5825,7 +5825,7 @@
       <c r="N170" s="5"/>
       <c r="O170" s="5"/>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>10</v>
       </c>
@@ -5856,7 +5856,7 @@
       <c r="N171" s="5"/>
       <c r="O171" s="5"/>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>12</v>
       </c>
@@ -5887,7 +5887,7 @@
       <c r="N172" s="5"/>
       <c r="O172" s="5"/>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>12</v>
       </c>
@@ -5918,7 +5918,7 @@
       <c r="N173" s="5"/>
       <c r="O173" s="5"/>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>12</v>
       </c>
@@ -5949,7 +5949,7 @@
       <c r="N174" s="5"/>
       <c r="O174" s="5"/>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>12</v>
       </c>
@@ -5980,7 +5980,7 @@
       <c r="N175" s="5"/>
       <c r="O175" s="5"/>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>12</v>
       </c>
@@ -6011,7 +6011,7 @@
       <c r="N176" s="5"/>
       <c r="O176" s="5"/>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>12</v>
       </c>
@@ -6042,7 +6042,7 @@
       <c r="N177" s="5"/>
       <c r="O177" s="5"/>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>12</v>
       </c>
@@ -6073,7 +6073,7 @@
       <c r="N178" s="5"/>
       <c r="O178" s="5"/>
     </row>
-    <row r="179" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>58</v>
       </c>
@@ -6104,7 +6104,7 @@
       <c r="N179" s="5"/>
       <c r="O179" s="5"/>
     </row>
-    <row r="180" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>58</v>
       </c>
@@ -6135,7 +6135,7 @@
       <c r="N180" s="5"/>
       <c r="O180" s="5"/>
     </row>
-    <row r="181" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>58</v>
       </c>
@@ -6166,7 +6166,7 @@
       <c r="N181" s="5"/>
       <c r="O181" s="5"/>
     </row>
-    <row r="182" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7" t="s">
         <v>69</v>
       </c>
@@ -6197,7 +6197,7 @@
       <c r="N182" s="5"/>
       <c r="O182" s="5"/>
     </row>
-    <row r="183" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>69</v>
       </c>
@@ -6228,7 +6228,7 @@
       <c r="N183" s="5"/>
       <c r="O183" s="5"/>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>69</v>
       </c>
@@ -6259,7 +6259,7 @@
       <c r="N184" s="5"/>
       <c r="O184" s="5"/>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>69</v>
       </c>
@@ -6290,7 +6290,7 @@
       <c r="N185" s="5"/>
       <c r="O185" s="5"/>
     </row>
-    <row r="186" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="7" t="s">
         <v>14</v>
       </c>
@@ -6321,7 +6321,7 @@
       <c r="N186" s="5"/>
       <c r="O186" s="5"/>
     </row>
-    <row r="187" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>14</v>
       </c>
@@ -6352,7 +6352,7 @@
       <c r="N187" s="5"/>
       <c r="O187" s="5"/>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>14</v>
       </c>
@@ -6383,7 +6383,7 @@
       <c r="N188" s="5"/>
       <c r="O188" s="5"/>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" s="7" t="s">
         <v>72</v>
       </c>
@@ -6414,7 +6414,7 @@
       <c r="N189" s="5"/>
       <c r="O189" s="5"/>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>72</v>
       </c>
@@ -6445,7 +6445,7 @@
       <c r="N190" s="5"/>
       <c r="O190" s="5"/>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>72</v>
       </c>
@@ -6476,7 +6476,7 @@
       <c r="N191" s="5"/>
       <c r="O191" s="5"/>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>72</v>
       </c>
@@ -6507,7 +6507,7 @@
       <c r="N192" s="5"/>
       <c r="O192" s="5"/>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>72</v>
       </c>
@@ -6538,7 +6538,7 @@
       <c r="N193" s="5"/>
       <c r="O193" s="5"/>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>72</v>
       </c>
@@ -6569,7 +6569,7 @@
       <c r="N194" s="5"/>
       <c r="O194" s="5"/>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>72</v>
       </c>
@@ -6600,7 +6600,7 @@
       <c r="N195" s="5"/>
       <c r="O195" s="5"/>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>72</v>
       </c>
@@ -6631,7 +6631,7 @@
       <c r="N196" s="5"/>
       <c r="O196" s="5"/>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>72</v>
       </c>
@@ -6662,7 +6662,7 @@
       <c r="N197" s="5"/>
       <c r="O197" s="5"/>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>72</v>
       </c>
@@ -6693,7 +6693,7 @@
       <c r="N198" s="5"/>
       <c r="O198" s="5"/>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>72</v>
       </c>
@@ -6724,7 +6724,7 @@
       <c r="N199" s="5"/>
       <c r="O199" s="5"/>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>72</v>
       </c>
@@ -6755,7 +6755,7 @@
       <c r="N200" s="5"/>
       <c r="O200" s="5"/>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>72</v>
       </c>
@@ -6786,7 +6786,7 @@
       <c r="N201" s="5"/>
       <c r="O201" s="5"/>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>72</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="N202" s="5"/>
       <c r="O202" s="5"/>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>72</v>
       </c>
@@ -6848,7 +6848,7 @@
       <c r="N203" s="5"/>
       <c r="O203" s="5"/>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>72</v>
       </c>
@@ -6879,7 +6879,7 @@
       <c r="N204" s="5"/>
       <c r="O204" s="5"/>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>72</v>
       </c>
@@ -6910,7 +6910,7 @@
       <c r="N205" s="5"/>
       <c r="O205" s="5"/>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>72</v>
       </c>
@@ -6941,7 +6941,7 @@
       <c r="N206" s="5"/>
       <c r="O206" s="5"/>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>72</v>
       </c>
@@ -6972,7 +6972,7 @@
       <c r="N207" s="5"/>
       <c r="O207" s="5"/>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>72</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="N208" s="5"/>
       <c r="O208" s="5"/>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" s="7" t="s">
         <v>9</v>
       </c>
@@ -7034,7 +7034,7 @@
       <c r="N209" s="5"/>
       <c r="O209" s="5"/>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>9</v>
       </c>
@@ -7065,7 +7065,7 @@
       <c r="N210" s="5"/>
       <c r="O210" s="5"/>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>58</v>
       </c>
@@ -7096,7 +7096,7 @@
       <c r="N211" s="5"/>
       <c r="O211" s="5"/>
     </row>
-    <row r="212" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>58</v>
       </c>
@@ -7127,7 +7127,7 @@
       <c r="N212" s="5"/>
       <c r="O212" s="5"/>
     </row>
-    <row r="213" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>12</v>
       </c>
@@ -7158,7 +7158,7 @@
       <c r="N213" s="5"/>
       <c r="O213" s="5"/>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>10</v>
       </c>
@@ -7190,7 +7190,7 @@
       <c r="N214" s="5"/>
       <c r="O214" s="5"/>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>10</v>
       </c>
@@ -7222,7 +7222,7 @@
       <c r="N215" s="5"/>
       <c r="O215" s="5"/>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" s="7" t="s">
         <v>22</v>
       </c>
@@ -7253,7 +7253,7 @@
       <c r="N216" s="5"/>
       <c r="O216" s="5"/>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>22</v>
       </c>
@@ -7284,7 +7284,7 @@
       <c r="N217" s="5"/>
       <c r="O217" s="5"/>
     </row>
-    <row r="218" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>22</v>
       </c>
@@ -7315,7 +7315,7 @@
       <c r="N218" s="5"/>
       <c r="O218" s="5"/>
     </row>
-    <row r="219" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>22</v>
       </c>
@@ -7347,7 +7347,7 @@
       <c r="N219" s="5"/>
       <c r="O219" s="5"/>
     </row>
-    <row r="220" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>22</v>
       </c>
@@ -7371,7 +7371,7 @@
       <c r="N220" s="5"/>
       <c r="O220" s="5"/>
     </row>
-    <row r="221" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>23</v>
       </c>
@@ -7402,7 +7402,7 @@
       <c r="N221" s="5"/>
       <c r="O221" s="5"/>
     </row>
-    <row r="222" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>23</v>
       </c>
@@ -7433,7 +7433,7 @@
       <c r="N222" s="5"/>
       <c r="O222" s="5"/>
     </row>
-    <row r="223" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>23</v>
       </c>
@@ -7459,7 +7459,7 @@
       <c r="N223" s="5"/>
       <c r="O223" s="5"/>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>84</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>45862</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>22</v>
       </c>
@@ -7517,7 +7517,7 @@
         <v>45919</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>9</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>45904</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>9</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>9</v>
       </c>
@@ -7602,7 +7602,7 @@
       </c>
       <c r="I228" s="2"/>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>58</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>45924</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>58</v>
       </c>
@@ -7662,7 +7662,7 @@
         <v>45957</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>45925</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>9</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>9</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>45912</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>93</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>93</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>93</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>95</v>
       </c>
@@ -7873,7 +7873,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>95</v>
       </c>
@@ -7921,43 +7921,43 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>84904</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>51512</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>49667</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>SUM(A1:A3)</f>
         <v>186083</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>122202733732</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>126971710115</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <f>A7-A6</f>
         <v>4768976383</v>

</xml_diff>